<commit_message>
Roughly finished v0.1 of the sccenarios
</commit_message>
<xml_diff>
--- a/analysis/scenarios.xlsx
+++ b/analysis/scenarios.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benjamin.FONTANA\Documents\GitHub\ProjetWeb\Web-Observation\analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mon\Documents\Github\ProjetWeb\Web-Observation\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F7C0F7B-7C04-445C-9E44-1F4C5C77D9B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16350" windowHeight="8385"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="58">
   <si>
     <t>Action user</t>
   </si>
@@ -190,12 +191,21 @@
   </si>
   <si>
     <t>cancel</t>
+  </si>
+  <si>
+    <t>view</t>
+  </si>
+  <si>
+    <t>click son a publication link</t>
+  </si>
+  <si>
+    <t>Returns the correct publication</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -477,22 +487,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -513,27 +528,22 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -815,14 +825,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L69"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B72" activeCellId="1" sqref="C70 B72:C75"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.28515625" customWidth="1"/>
     <col min="2" max="2" width="41.7109375" customWidth="1"/>
@@ -832,11 +842,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="25"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="13"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -845,21 +855,21 @@
       <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -873,7 +883,7 @@
       <c r="F3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
-      <c r="J3" s="18"/>
+      <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -885,7 +895,7 @@
       <c r="F4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="18"/>
+      <c r="J4" s="3"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -899,7 +909,7 @@
       <c r="F5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-      <c r="J5" s="18"/>
+      <c r="J5" s="3"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -911,7 +921,7 @@
       <c r="F6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="18"/>
+      <c r="J6" s="3"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
@@ -919,9 +929,9 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C8" s="2" t="s">
@@ -929,49 +939,49 @@
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
+      <c r="A9" s="3"/>
       <c r="C9" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="18"/>
+      <c r="C10" s="3"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
-      <c r="B11" s="18"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
       <c r="C11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="18"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
@@ -983,34 +993,34 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="18"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
     </row>
     <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="23" t="s">
+      <c r="A13" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="24"/>
-      <c r="C13" s="25"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="13"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="18"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
     </row>
     <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="7" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="1"/>
@@ -1019,9 +1029,9 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="18"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -1036,9 +1046,9 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="18"/>
-      <c r="L15" s="18"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1051,9 +1061,9 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="18"/>
-      <c r="L16" s="18"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
@@ -1069,35 +1079,35 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="18"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19" t="s">
+      <c r="B18" s="4"/>
+      <c r="C18" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="18"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="19"/>
+      <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C19" s="1"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="18"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
@@ -1105,12 +1115,12 @@
       <c r="C20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="18"/>
-      <c r="L20" s="18"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
@@ -1124,9 +1134,9 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="18"/>
-      <c r="L21" s="18"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
@@ -1140,9 +1150,9 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="18"/>
-      <c r="L22" s="18"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
     </row>
     <row r="23" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
@@ -1152,34 +1162,34 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="18"/>
-      <c r="L23" s="18"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
     </row>
     <row r="24" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="15" t="s">
+      <c r="A24" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="16"/>
-      <c r="C24" s="17"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="10"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
-      <c r="J24" s="18"/>
-      <c r="K24" s="18"/>
-      <c r="L24" s="18"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
     </row>
     <row r="25" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="20" t="s">
+      <c r="A25" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B25" s="21" t="s">
+      <c r="B25" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="22" t="s">
+      <c r="C25" s="7" t="s">
         <v>2</v>
       </c>
       <c r="D25" s="1"/>
@@ -1188,9 +1198,9 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
-      <c r="J25" s="18"/>
-      <c r="K25" s="18"/>
-      <c r="L25" s="18"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
@@ -1205,9 +1215,9 @@
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="18"/>
-      <c r="L26" s="18"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
     </row>
     <row r="27" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
@@ -1219,34 +1229,34 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
-      <c r="J27" s="18"/>
-      <c r="K27" s="18"/>
-      <c r="L27" s="18"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
     </row>
     <row r="28" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="15" t="s">
+      <c r="A28" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="16"/>
-      <c r="C28" s="17"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="10"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
-      <c r="J28" s="18"/>
-      <c r="K28" s="18"/>
-      <c r="L28" s="18"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
     </row>
     <row r="29" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="20" t="s">
+      <c r="A29" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B29" s="21" t="s">
+      <c r="B29" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C29" s="22" t="s">
+      <c r="C29" s="7" t="s">
         <v>2</v>
       </c>
       <c r="D29" s="1"/>
@@ -1255,9 +1265,9 @@
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
-      <c r="J29" s="18"/>
-      <c r="K29" s="18"/>
-      <c r="L29" s="18"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
@@ -1272,9 +1282,9 @@
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
-      <c r="J30" s="18"/>
-      <c r="K30" s="18"/>
-      <c r="L30" s="18"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
@@ -1287,9 +1297,9 @@
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
-      <c r="J31" s="18"/>
-      <c r="K31" s="18"/>
-      <c r="L31" s="18"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
@@ -1305,9 +1315,9 @@
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
-      <c r="J32" s="18"/>
-      <c r="K32" s="18"/>
-      <c r="L32" s="18"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
@@ -1321,79 +1331,79 @@
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
-      <c r="J33" s="18"/>
-      <c r="K33" s="18"/>
-      <c r="L33" s="18"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="18"/>
+      <c r="A34" s="3"/>
       <c r="C34" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
-      <c r="H34" s="18"/>
-      <c r="I34" s="18"/>
-      <c r="J34" s="18"/>
-      <c r="K34" s="18"/>
-      <c r="L34" s="18"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="18"/>
-      <c r="B35" s="18"/>
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
       <c r="C35" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
-      <c r="H35" s="18"/>
-      <c r="I35" s="18"/>
-      <c r="J35" s="18"/>
-      <c r="K35" s="18"/>
-      <c r="L35" s="18"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
     </row>
     <row r="36" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="18"/>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
-      <c r="H36" s="18"/>
-      <c r="I36" s="18"/>
-      <c r="J36" s="18"/>
-      <c r="K36" s="18"/>
-      <c r="L36" s="18"/>
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
     </row>
     <row r="37" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="15" t="s">
+      <c r="A37" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B37" s="16"/>
-      <c r="C37" s="17"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="10"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
-      <c r="J37" s="18"/>
-      <c r="K37" s="18"/>
-      <c r="L37" s="18"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
     </row>
     <row r="38" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="20" t="s">
+      <c r="A38" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B38" s="21" t="s">
+      <c r="B38" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C38" s="22" t="s">
+      <c r="C38" s="7" t="s">
         <v>2</v>
       </c>
       <c r="D38" s="1"/>
@@ -1402,9 +1412,9 @@
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
-      <c r="J38" s="18"/>
-      <c r="K38" s="18"/>
-      <c r="L38" s="18"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
@@ -1477,20 +1487,20 @@
     </row>
     <row r="49" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="50" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="15" t="s">
+      <c r="A50" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B50" s="16"/>
-      <c r="C50" s="17"/>
+      <c r="B50" s="9"/>
+      <c r="C50" s="10"/>
     </row>
     <row r="51" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="20" t="s">
+      <c r="A51" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B51" s="21" t="s">
+      <c r="B51" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C51" s="22" t="s">
+      <c r="C51" s="7" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1556,20 +1566,20 @@
     </row>
     <row r="62" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="63" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="15" t="s">
+      <c r="A63" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B63" s="16"/>
-      <c r="C63" s="17"/>
+      <c r="B63" s="9"/>
+      <c r="C63" s="10"/>
     </row>
     <row r="64" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="20" t="s">
+      <c r="A64" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B64" s="21" t="s">
+      <c r="B64" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C64" s="22" t="s">
+      <c r="C64" s="7" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1605,8 +1615,43 @@
         <v>54</v>
       </c>
     </row>
+    <row r="70" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="71" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B71" s="9"/>
+      <c r="C71" s="10"/>
+    </row>
+    <row r="72" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B74" s="1"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="1"/>
+      <c r="C75" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="A71:C71"/>
     <mergeCell ref="A50:C50"/>
     <mergeCell ref="A63:C63"/>
     <mergeCell ref="A1:C1"/>
@@ -1621,87 +1666,87 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="17"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="12" t="s">
+      <c r="B2" s="18"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="13"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="12" t="s">
+      <c r="E2" s="18"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="13"/>
-      <c r="I2" s="14"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="19"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="9" t="s">
+      <c r="B3" s="15"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="9" t="s">
+      <c r="E3" s="15"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="10"/>
-      <c r="I3" s="11"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="16"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="3" t="s">
+      <c r="A4" s="23"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="5"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="25"/>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="6" t="s">
+      <c r="A5" s="20"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="7"/>
-      <c r="I5" s="8"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="13">

</xml_diff>